<commit_message>
Tabela de Testes (VBA) criada - Correção no algoritmo de geração de trajetória
</commit_message>
<xml_diff>
--- a/TestTable.xlsx
+++ b/TestTable.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="7635" windowHeight="6975"/>
   </bookViews>
@@ -16,22 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>v_star</t>
-  </si>
-  <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>v0</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>t1</t>
   </si>
@@ -42,24 +27,124 @@
     <t>t3</t>
   </si>
   <si>
-    <t>a02_2J</t>
-  </si>
-  <si>
-    <t>a_lim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">t2 </t>
+    <t>Initial Acceleration (a0)</t>
+  </si>
+  <si>
+    <t>initial Velocity (v0)</t>
+  </si>
+  <si>
+    <t>Maximum Deceleration (d)</t>
+  </si>
+  <si>
+    <t>Initial Position (s0)</t>
+  </si>
+  <si>
+    <t>Desired Jerk (J)</t>
+  </si>
+  <si>
+    <t>v*</t>
+  </si>
+  <si>
+    <r>
+      <t>(a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/(2J)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lim</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,9 +172,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,122 +477,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J14"/>
+  <sheetPr codeName="Plan1"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>-5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <f>(C4-C2)/C5</f>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <f>C2^2/(2*C5*C4) - C2/C5 - C3/C4</f>
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <f xml:space="preserve"> C2^2/(2*C5) - C4^2/C5</f>
+        <v>-5.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="G4">
-        <f>C4/C5 + G3</f>
-        <v>1.7833333333333332</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>8</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>(C4-C2)/C5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C7">
-        <f>C2^2/(2*C5)</f>
-        <v>2.5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="e">
-        <f>(C9-C2)/C5</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
         <v>0</v>
       </c>
-      <c r="C8">
-        <f xml:space="preserve"> C2^2/(2*C5) - C4^2/C5</f>
-        <v>-4.7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="e">
-        <f>C9/C5</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="e">
-        <f>SQRT((C2^2/2) - C5*C3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D9">
-        <f>SQRT((C2^2/2) + C5*C3)</f>
-        <v>6.1237243569579451</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f>C2^2/(2*C5*C4) - C2/C5 - C3/C4</f>
+        <v>-1.3666666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f>C4/C5 + F7</f>
+        <v>-0.16666666666666674</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -519,6 +599,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>